<commit_message>
update leave date after add test result
</commit_message>
<xml_diff>
--- a/scriptDatabase/KetQuaXetNghiemvv20-10-2021.xlsx
+++ b/scriptDatabase/KetQuaXetNghiemvv20-10-2021.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIT\HK5-2020-2021\PhuongPhapPhatTrienPhanMemHuongDoiTuong-SE100.M12\Project\QuanLyKhuCachLy\scriptDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFC30E0-3FEA-4C75-8879-A34EF34764B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{64F8E407-D7D9-4A01-8D03-8DB1D60843B8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kết quả</t>
   </si>
@@ -45,13 +44,13 @@
     <t>Ngày xét nghiệm</t>
   </si>
   <si>
-    <t>âm tính</t>
+    <t>dương tính</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +85,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,19 +396,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34051878-AA99-4B20-908F-DFA540EB57BF}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -420,81 +419,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>44291</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>166</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>168</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>170</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>171</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44297</v>
+        <v>44540</v>
       </c>
     </row>
   </sheetData>
@@ -503,6 +436,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x0101003008510C1118BA4F933B65825EE70E70" ma:contentTypeVersion="10" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="3ae2b50c9ec3c34be56549c49b211cc0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="77782a45-0a80-4861-8bd4-635a88548cdf" xmlns:ns3="ba774fb5-2cf8-465a-a24b-3e0d6c5ac152" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab02b8847b1880d3d80338b07611e388" ns2:_="" ns3:_="">
     <xsd:import namespace="77782a45-0a80-4861-8bd4-635a88548cdf"/>
@@ -705,29 +653,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DABB910-5AAA-4151-B511-2885EFEB676A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BE1B385-EA79-4D61-AD30-C3D09851FE3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BE1B385-EA79-4D61-AD30-C3D09851FE3A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5A458E-78F7-41F0-844E-B441A16D5A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5A458E-78F7-41F0-844E-B441A16D5A49}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DABB910-5AAA-4151-B511-2885EFEB676A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="77782a45-0a80-4861-8bd4-635a88548cdf"/>
+    <ds:schemaRef ds:uri="ba774fb5-2cf8-465a-a24b-3e0d6c5ac152"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add confirm dialog for update leave date after insert test result throught execel file
</commit_message>
<xml_diff>
--- a/scriptDatabase/KetQuaXetNghiemvv20-10-2021.xlsx
+++ b/scriptDatabase/KetQuaXetNghiemvv20-10-2021.xlsx
@@ -44,7 +44,7 @@
     <t>Ngày xét nghiệm</t>
   </si>
   <si>
-    <t>dương tính</t>
+    <t>âm tính</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>44540</v>
+        <v>44541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>